<commit_message>
Update changes as required
</commit_message>
<xml_diff>
--- a/UI3/output/log2.xlsx
+++ b/UI3/output/log2.xlsx
@@ -31,13 +31,13 @@
     <t>time</t>
   </si>
   <si>
-    <t>mindepth</t>
+    <t>Min depth</t>
   </si>
   <si>
-    <t>maxdepth</t>
+    <t>Max depth</t>
   </si>
   <si>
-    <t>avgdepth</t>
+    <t>Average depth</t>
   </si>
   <si>
     <t>errmsg</t>
@@ -235,7 +235,7 @@
     <t>2018-5-25-11-3</t>
   </si>
   <si>
-    <t>sync_rate</t>
+    <t>Sync rate</t>
   </si>
   <si>
     <t>2018-4-11-14-24</t>
@@ -334,10 +334,10 @@
     <t>4th straight right elbow angle</t>
   </si>
   <si>
-    <t>average right hand push down angle</t>
+    <t>Average right hand push down angle</t>
   </si>
   <si>
-    <t>average right hand straight angle</t>
+    <t>Average right hand straight angle</t>
   </si>
   <si>
     <t>1st lower left elbow angle</t>
@@ -364,10 +364,10 @@
     <t>4th straight left elbow angle</t>
   </si>
   <si>
-    <t>average left hand push down angle</t>
+    <t>Average left hand push down angle</t>
   </si>
   <si>
-    <t>average left hand straight angle</t>
+    <t>Average left hand straight angle</t>
   </si>
   <si>
     <t>2018-4-5-17-8</t>
@@ -499,10 +499,10 @@
     <t>4th right hand angle (T-pose)</t>
   </si>
   <si>
-    <t>average right hand angle (H-close)</t>
+    <t>Average right hand angle (H-close)</t>
   </si>
   <si>
-    <t>average right hand angle (T-pose)</t>
+    <t>Average right hand angle (T-pose)</t>
   </si>
   <si>
     <t>1st left hand angle (H-close)</t>
@@ -529,10 +529,10 @@
     <t>4th left hand angle (T-pose)</t>
   </si>
   <si>
-    <t>average left hand angle (H-close)</t>
+    <t>Average left hand angle (H-close)</t>
   </si>
   <si>
-    <t>average left hand angle (T-pose)</t>
+    <t>Average left hand angle (T-pose)</t>
   </si>
   <si>
     <t>2018-4-5-16-57</t>
@@ -679,7 +679,7 @@
     <t>Min hold time</t>
   </si>
   <si>
-    <t>average hold time</t>
+    <t>Average hold time</t>
   </si>
   <si>
     <t>2018-4-5-18-20</t>
@@ -18420,7 +18420,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -19396,16 +19396,16 @@
         <v>12</v>
       </c>
       <c r="D35" t="s" s="7">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E35" s="8">
-        <v>50.0602463054187</v>
+        <v>51.28095901544177</v>
       </c>
       <c r="F35" s="8">
-        <v>75.76999627976187</v>
+        <v>80.54771835061487</v>
       </c>
       <c r="G35" s="8">
-        <v>64.38746706218842</v>
+        <v>62.75439057845091</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -19422,16 +19422,16 @@
         <v>12</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E36" s="8">
-        <v>41.1863085656189</v>
+        <v>31.08272611169162</v>
       </c>
       <c r="F36" s="8">
-        <v>60.31189743138633</v>
+        <v>65.78995610870609</v>
       </c>
       <c r="G36" s="8">
-        <v>50.74910299850262</v>
+        <v>49.68287335675945</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -19448,176 +19448,20 @@
         <v>12</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E37" s="8">
-        <v>33.88205128205126</v>
+        <v>20.85618160307601</v>
       </c>
       <c r="F37" s="8">
-        <v>100.9295206331651</v>
+        <v>41.37243423742673</v>
       </c>
       <c r="G37" s="8">
-        <v>71.84454371050415</v>
+        <v>33.29692690181689</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" ht="15" customHeight="1">
-      <c r="A38" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B38" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s" s="7">
-        <v>91</v>
-      </c>
-      <c r="E38" s="8">
-        <v>46.27505285412261</v>
-      </c>
-      <c r="F38" s="8">
-        <v>91.79676079734216</v>
-      </c>
-      <c r="G38" s="8">
-        <v>65.16081120940149</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B39" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C39" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s" s="7">
-        <v>92</v>
-      </c>
-      <c r="E39" s="8">
-        <v>31.47003246753246</v>
-      </c>
-      <c r="F39" s="8">
-        <v>85.46485779666554</v>
-      </c>
-      <c r="G39" s="8">
-        <v>60.26271414098727</v>
-      </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" ht="15" customHeight="1">
-      <c r="A40" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C40" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s" s="7">
-        <v>93</v>
-      </c>
-      <c r="E40" s="8">
-        <v>30.90576466307188</v>
-      </c>
-      <c r="F40" s="8">
-        <v>83.17362324730743</v>
-      </c>
-      <c r="G40" s="8">
-        <v>59.60766650460843</v>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" ht="15" customHeight="1">
-      <c r="A41" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B41" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C41" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D41" t="s" s="7">
-        <v>94</v>
-      </c>
-      <c r="E41" s="8">
-        <v>51.28095901544177</v>
-      </c>
-      <c r="F41" s="8">
-        <v>80.54771835061487</v>
-      </c>
-      <c r="G41" s="8">
-        <v>62.75439057845091</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B42" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C42" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D42" t="s" s="7">
-        <v>95</v>
-      </c>
-      <c r="E42" s="8">
-        <v>31.08272611169162</v>
-      </c>
-      <c r="F42" s="8">
-        <v>65.78995610870609</v>
-      </c>
-      <c r="G42" s="8">
-        <v>49.68287335675945</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C43" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="D43" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="E43" s="8">
-        <v>20.85618160307601</v>
-      </c>
-      <c r="F43" s="8">
-        <v>41.37243423742673</v>
-      </c>
-      <c r="G43" s="8">
-        <v>33.29692690181689</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>